<commit_message>
Fix case to avoid a coouple warnings.
</commit_message>
<xml_diff>
--- a/2019/com-20190714-simplified.xlsx
+++ b/2019/com-20190714-simplified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/mac/results/2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A087AB88-24EF-0E43-BEF6-32519704E208}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D114CAA-EDAC-0E4D-ACE7-5799EF1C73F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="460" windowWidth="16120" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t xml:space="preserve"> AS</t>
   </si>
   <si>
-    <t xml:space="preserve"> RICK SELLNER</t>
-  </si>
-  <si>
     <t xml:space="preserve"> DAVE BEIREIS</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t xml:space="preserve"> BSP</t>
   </si>
   <si>
-    <t xml:space="preserve"> QUINCY TAMBO</t>
-  </si>
-  <si>
     <t xml:space="preserve"> TREVOR ROWE</t>
   </si>
   <si>
@@ -302,9 +296,6 @@
     <t xml:space="preserve"> CARSON TURNQUIST</t>
   </si>
   <si>
-    <t xml:space="preserve"> JON PIERCE-RUHLAND</t>
-  </si>
-  <si>
     <t xml:space="preserve"> XP</t>
   </si>
   <si>
@@ -339,6 +330,15 @@
   </si>
   <si>
     <t>final_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jon Pierce-Ruhland</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rick Sellner</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quincy Tambo</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1239,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1251,19 +1253,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1308,7 +1310,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="D6" s="6">
         <v>63.728000000000002</v>
@@ -1320,7 +1322,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="6">
         <v>64.680999999999997</v>
@@ -1332,7 +1334,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="6">
         <v>65.757000000000005</v>
@@ -1344,7 +1346,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="6">
         <v>72.006</v>
@@ -1353,10 +1355,10 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
       </c>
       <c r="D11" s="6">
         <v>63.774000000000001</v>
@@ -1365,10 +1367,10 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="6">
         <v>65.581000000000003</v>
@@ -1377,10 +1379,10 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="6">
         <v>65.683000000000007</v>
@@ -1389,10 +1391,10 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="6">
         <v>67.135999999999996</v>
@@ -1401,10 +1403,10 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
       </c>
       <c r="D16" s="6">
         <v>65.131</v>
@@ -1413,10 +1415,10 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
         <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
       </c>
       <c r="D18" s="7">
         <v>64.709999999999994</v>
@@ -1425,10 +1427,10 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="6">
         <v>65.268000000000001</v>
@@ -1437,10 +1439,10 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="6">
         <v>66.024000000000001</v>
@@ -1449,10 +1451,10 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="6">
         <v>67.292000000000002</v>
@@ -1461,10 +1463,10 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="6">
         <v>94.971999999999994</v>
@@ -1473,10 +1475,10 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
         <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>23</v>
       </c>
       <c r="D24" s="6">
         <v>69.347999999999999</v>
@@ -1485,10 +1487,10 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
         <v>24</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
       </c>
       <c r="D26" s="6">
         <v>62.819000000000003</v>
@@ -1497,10 +1499,10 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="6">
         <v>68.262</v>
@@ -1509,10 +1511,10 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="6">
         <v>70.147000000000006</v>
@@ -1524,10 +1526,10 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D30" s="6">
         <v>68.263000000000005</v>
@@ -1536,10 +1538,10 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="D32" s="6">
         <v>63.018999999999998</v>
@@ -1548,10 +1550,10 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
         <v>28</v>
-      </c>
-      <c r="C33" t="s">
-        <v>30</v>
       </c>
       <c r="D33" s="6">
         <v>65.823999999999998</v>
@@ -1560,10 +1562,10 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D34" s="6">
         <v>68.631</v>
@@ -1572,10 +1574,10 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D35" s="6">
         <v>72.912999999999997</v>
@@ -1587,10 +1589,10 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D37" s="6">
         <v>66.850999999999999</v>
@@ -1602,10 +1604,10 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D39" s="6">
         <v>64.581000000000003</v>
@@ -1614,10 +1616,10 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
         <v>33</v>
-      </c>
-      <c r="C40" t="s">
-        <v>35</v>
       </c>
       <c r="D40" s="6">
         <v>65.295000000000002</v>
@@ -1626,10 +1628,10 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D41" s="6">
         <v>65.638000000000005</v>
@@ -1641,10 +1643,10 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D44" s="6">
         <v>59.719000000000001</v>
@@ -1653,10 +1655,10 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" t="s">
         <v>37</v>
-      </c>
-      <c r="C45" t="s">
-        <v>39</v>
       </c>
       <c r="D45" s="6">
         <v>63.021000000000001</v>
@@ -1665,10 +1667,10 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D46" s="6">
         <v>63.621000000000002</v>
@@ -1677,10 +1679,10 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D47" s="6">
         <v>63.889000000000003</v>
@@ -1689,10 +1691,10 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D48" s="6">
         <v>65.182000000000002</v>
@@ -1701,10 +1703,10 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C49" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D49" s="6">
         <v>69.561000000000007</v>
@@ -1713,10 +1715,10 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D50" s="6">
         <v>70.807000000000002</v>
@@ -1725,10 +1727,10 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D51" s="6">
         <v>71.174000000000007</v>
@@ -1737,10 +1739,10 @@
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D53" s="6">
         <v>66.471999999999994</v>
@@ -1749,10 +1751,10 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" t="s">
         <v>46</v>
-      </c>
-      <c r="C54" t="s">
-        <v>48</v>
       </c>
       <c r="D54" s="6">
         <v>67.468000000000004</v>
@@ -1761,10 +1763,10 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D55" s="6">
         <v>70.418999999999997</v>
@@ -1773,10 +1775,10 @@
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D57" s="6">
         <v>62.697000000000003</v>
@@ -1785,10 +1787,10 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
         <v>50</v>
-      </c>
-      <c r="C58" t="s">
-        <v>52</v>
       </c>
       <c r="D58" s="6">
         <v>64.617000000000004</v>
@@ -1797,10 +1799,10 @@
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D59" s="6">
         <v>67.093000000000004</v>
@@ -1809,10 +1811,10 @@
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D60" s="6">
         <v>67.838999999999999</v>
@@ -1821,10 +1823,10 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C62" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D62" s="6">
         <v>64.134</v>
@@ -1833,10 +1835,10 @@
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" t="s">
         <v>55</v>
-      </c>
-      <c r="C63" t="s">
-        <v>57</v>
       </c>
       <c r="D63" s="6">
         <v>66.632000000000005</v>
@@ -1848,10 +1850,10 @@
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C65" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D65" s="6">
         <v>65.093000000000004</v>
@@ -1860,10 +1862,10 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C66" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D66" s="6">
         <v>66.917000000000002</v>
@@ -1875,10 +1877,10 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D68" s="6">
         <v>61.554000000000002</v>
@@ -1887,10 +1889,10 @@
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C69" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D69" s="6">
         <v>68.614000000000004</v>
@@ -1902,10 +1904,10 @@
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D71" s="6">
         <v>61.427999999999997</v>
@@ -1914,10 +1916,10 @@
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C72" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D72" s="6">
         <v>63.523000000000003</v>
@@ -1929,10 +1931,10 @@
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C74" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D74" s="6">
         <v>65.450999999999993</v>
@@ -1944,10 +1946,10 @@
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C76" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D76" s="6">
         <v>67.745999999999995</v>
@@ -1955,13 +1957,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B78" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C78" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E78" s="6">
         <v>49.923000000000002</v>
@@ -1969,13 +1971,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B79" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C79" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E79" s="6">
         <v>51.122999999999998</v>
@@ -1983,13 +1985,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B80" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C80" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E80" s="7">
         <v>52.1</v>
@@ -1997,13 +1999,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B81" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C81" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E81" s="7">
         <v>52.728999999999999</v>
@@ -2011,13 +2013,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C82" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E82" s="6">
         <v>53.021000000000001</v>
@@ -2025,13 +2027,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C83" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E83" s="6">
         <v>53.494</v>
@@ -2039,13 +2041,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B84" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C84" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E84" s="6">
         <v>53.899000000000001</v>
@@ -2053,13 +2055,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C85" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E85" s="6">
         <v>54.232999999999997</v>
@@ -2067,13 +2069,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C86" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E86" s="7">
         <v>54.259</v>
@@ -2081,13 +2083,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C87" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E87" s="6">
         <v>54.371000000000002</v>
@@ -2095,13 +2097,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C88" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E88" s="6">
         <v>54.750999999999998</v>
@@ -2109,13 +2111,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C89" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E89" s="6">
         <v>55.125999999999998</v>
@@ -2123,13 +2125,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C90" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E90" s="6">
         <v>56.142000000000003</v>
@@ -2140,13 +2142,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E92" s="7">
         <v>48.92</v>
@@ -2154,13 +2156,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B93" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C93" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E93" s="7">
         <v>49.151000000000003</v>
@@ -2168,13 +2170,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B94" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C94" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E94" s="6">
         <v>49.561</v>
@@ -2182,13 +2184,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B95" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C95" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E95" s="6">
         <v>51.030999999999999</v>
@@ -2196,13 +2198,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B96" t="s">
         <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E96" s="6">
         <v>54.545000000000002</v>

</xml_diff>